<commit_message>
Update SEO taxonomy content, homepage copy direction, and keyword research v2 outputs
</commit_message>
<xml_diff>
--- a/seo/Product_Taxonomy_Nav.xlsx
+++ b/seo/Product_Taxonomy_Nav.xlsx
@@ -8,25 +8,940 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darshinipaul/Documents/Projects/alex-and-arms/seo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3B66E3-0196-9140-9288-E31F759F4FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB81BAEA-E387-8B42-B92E-2AFDDFAAE2EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Product Category Taxonomy" sheetId="1" r:id="rId1"/>
-    <sheet name="Brands" sheetId="2" r:id="rId2"/>
-    <sheet name="Browse by Room" sheetId="3" r:id="rId3"/>
-    <sheet name="Top Nav" sheetId="5" r:id="rId4"/>
+    <sheet name="SEO Master List" sheetId="1" r:id="rId1"/>
+    <sheet name="SEO Master List-working" sheetId="2" r:id="rId2"/>
+    <sheet name="Home_Copy" sheetId="7" r:id="rId3"/>
+    <sheet name="Product Category Taxonomy" sheetId="3" r:id="rId4"/>
+    <sheet name="Brands" sheetId="4" r:id="rId5"/>
+    <sheet name="Browse by Room" sheetId="5" r:id="rId6"/>
+    <sheet name="Top Nav" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Brands!$A$1:$B$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Brands!$A$1:$B$20</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="408">
+  <si>
+    <t>Page Type</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>Primary Keyword</t>
+  </si>
+  <si>
+    <t>Secondary Keywords</t>
+  </si>
+  <si>
+    <t>Meta Description</t>
+  </si>
+  <si>
+    <t>Browser Title</t>
+  </si>
+  <si>
+    <t>Slug</t>
+  </si>
+  <si>
+    <t>FAQs (Y/N)</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>L1 Product</t>
+  </si>
+  <si>
+    <t>Tiles</t>
+  </si>
+  <si>
+    <t>L2 Product</t>
+  </si>
+  <si>
+    <t>Vitrified Tiles</t>
+  </si>
+  <si>
+    <t>Ceramic Tiles</t>
+  </si>
+  <si>
+    <t>Floor Tiles</t>
+  </si>
+  <si>
+    <t>Wall Tiles</t>
+  </si>
+  <si>
+    <t>Sanitaryware &amp; Bathroom Fittings</t>
+  </si>
+  <si>
+    <t>Toilets and Water Closets</t>
+  </si>
+  <si>
+    <t>Urinals</t>
+  </si>
+  <si>
+    <t>Wash Basins</t>
+  </si>
+  <si>
+    <t>Taps &amp; Faucets</t>
+  </si>
+  <si>
+    <t>Bath &amp; Wellness</t>
+  </si>
+  <si>
+    <t>Bathroom Accessories</t>
+  </si>
+  <si>
+    <t>Mirrors &amp; Cabinets</t>
+  </si>
+  <si>
+    <t>Water Heaters</t>
+  </si>
+  <si>
+    <t>Floor Drains</t>
+  </si>
+  <si>
+    <t>Differently-Abled Bath Products</t>
+  </si>
+  <si>
+    <t>Public Restroom Solutions</t>
+  </si>
+  <si>
+    <t>Kitchen Appliances &amp; Sinks</t>
+  </si>
+  <si>
+    <t>Sinks</t>
+  </si>
+  <si>
+    <t>Chimneys</t>
+  </si>
+  <si>
+    <t>Kitchen Sinks &amp; Faucets</t>
+  </si>
+  <si>
+    <t>Other Appliances</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>GROHE</t>
+  </si>
+  <si>
+    <t>RAK Ceramics</t>
+  </si>
+  <si>
+    <t>AGL</t>
+  </si>
+  <si>
+    <t>Hindware</t>
+  </si>
+  <si>
+    <t>Carysil</t>
+  </si>
+  <si>
+    <t>Franke</t>
+  </si>
+  <si>
+    <t>Roff</t>
+  </si>
+  <si>
+    <t>Ardex Endura</t>
+  </si>
+  <si>
+    <t>AO Smith</t>
+  </si>
+  <si>
+    <t>Racold</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Bathroom Solutions</t>
+  </si>
+  <si>
+    <t>Kitchen Essentials</t>
+  </si>
+  <si>
+    <t>Outdoor &amp; Parking</t>
+  </si>
+  <si>
+    <t>Commercial Restrooms</t>
+  </si>
+  <si>
+    <t>Basic Details</t>
+  </si>
+  <si>
+    <t>SEO metadata</t>
+  </si>
+  <si>
+    <t>Optional Sections</t>
+  </si>
+  <si>
+    <t>Page Copy</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Meta Description (150 char)</t>
+  </si>
+  <si>
+    <t>FAQs needed (Y/N)</t>
+  </si>
+  <si>
+    <t>Hero banner title (h1)</t>
+  </si>
+  <si>
+    <t>Hero banner description</t>
+  </si>
+  <si>
+    <t>tile showroom chennai</t>
+  </si>
+  <si>
+    <t>vadapalani tiles showroom, ceramics chennai, bathroom fittings chennai, floor tiles chennai, kag tiles chennai, kitchen sink chennai, sanitaryware chennai</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Explore tiles, sanitaryware, faucets, and kitchen essentials at Alex &amp; Arms Ceramica in Chennai. Visit our showroom for trusted brands and guidance.</t>
+  </si>
+  <si>
+    <t>Tiles, Sanitaryware &amp; Faucets in Chennai | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Tiles, Sanitaryware &amp; Kitchen Solutions in Chennai</t>
+  </si>
+  <si>
+    <t>Explore tiles, sanitaryware, faucets, and kitchen essentials from trusted brands at Alex &amp; Arms Ceramica.</t>
+  </si>
+  <si>
+    <t>alex and arms ceramica</t>
+  </si>
+  <si>
+    <t>alex and arms ceramics, alex tiles, vadapalani tiles shop, chennai ceramics shop</t>
+  </si>
+  <si>
+    <t>Learn about Alex &amp; Arms Ceramica, our product categories, and trusted brand partnerships in Chennai for home and commercial spaces.</t>
+  </si>
+  <si>
+    <t>About Us | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/about</t>
+  </si>
+  <si>
+    <t>About Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>Learn how Alex &amp; Arms Ceramica supports customers with practical product guidance and curated brand options in Chennai.</t>
+  </si>
+  <si>
+    <t>tiles chennai</t>
+  </si>
+  <si>
+    <t>tile showroom chennai, athangudi tiles chennai, best tile shop in chennai, best tiles showroom in chennai, chennai tile shop, cool roof tiles chennai, cost of tiles in chennai, floor tiles chennai</t>
+  </si>
+  <si>
+    <t>Browse tiles at Alex &amp; Arms Ceramica in Chennai. Explore practical options across sizes, materials, and designs.</t>
+  </si>
+  <si>
+    <t>Tiles in Chennai | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/tiles</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Find floor and wall tile options across finishes, sizes, and styles for residential and commercial spaces.</t>
+  </si>
+  <si>
+    <t>vitrified tiles chennai</t>
+  </si>
+  <si>
+    <t>2x2 vitrified tiles in chennai, agl double charge vitrified tiles, rak double charge vitrified tiles price, vitrified tiles price chennai</t>
+  </si>
+  <si>
+    <t>Browse vitrified tiles at Alex &amp; Arms Ceramica in Chennai. Explore practical options across sizes, materials, and designs.</t>
+  </si>
+  <si>
+    <t>Vitrified Tiles | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/tiles/vitrified-tiles</t>
+  </si>
+  <si>
+    <t>Explore low-maintenance vitrified tile options suited for high-use areas with modern finishes and formats.</t>
+  </si>
+  <si>
+    <t>ceramic tiles chennai</t>
+  </si>
+  <si>
+    <t>agl ceramic tiles, ceramic tiles dealers in chennai, ceramic tiles price in chennai,  rk ceramic tiles</t>
+  </si>
+  <si>
+    <t>Browse ceramic tiles at Alex &amp; Arms Ceramica in Chennai. Explore practical options across sizes, materials, and designs.</t>
+  </si>
+  <si>
+    <t>Ceramic Tiles | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/tiles/ceramic-tiles</t>
+  </si>
+  <si>
+    <t>Browse ceramic tile options for walls and floors with versatile designs for everyday use.</t>
+  </si>
+  <si>
+    <t>floor tiles chennai</t>
+  </si>
+  <si>
+    <t>2x2 floor tiles price in chennai, 3d floor tiles price in chennai, agl floor tiles price, bathroom floor tiles chennai, best floor tiles in chennai, ceramic floor tiles price in chennai</t>
+  </si>
+  <si>
+    <t>Browse floor tiles at Alex &amp; Arms Ceramica in Chennai. Explore practical options across sizes, materials, and designs.</t>
+  </si>
+  <si>
+    <t>Floor Tiles | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/tiles/floor-tiles</t>
+  </si>
+  <si>
+    <t>Compare floor tile options designed for durability, easy upkeep, and style across living spaces.</t>
+  </si>
+  <si>
+    <t>wall tiles chennai</t>
+  </si>
+  <si>
+    <t>agl bathroom wall tiles, bathroom wall tiles price in chennai, exterior wall tiles chennai, foam wall tiles in chennai, kitchen wall tiles chennai, kitchen wall tiles design in chennai</t>
+  </si>
+  <si>
+    <t>Browse wall tiles at Alex &amp; Arms Ceramica in Chennai. Explore practical options across sizes, materials, and designs.</t>
+  </si>
+  <si>
+    <t>Wall Tiles | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/tiles/wall-tiles</t>
+  </si>
+  <si>
+    <t>Discover wall tile options that combine visual appeal with practical maintenance for kitchens and bathrooms.</t>
+  </si>
+  <si>
+    <t>bathroom fittings chennai</t>
+  </si>
+  <si>
+    <t>bathroom fittings showroom in chennai, best bathroom fittings in chennai, hindware sanitaryware chennai, hindware sanitaryware dealers in chennai</t>
+  </si>
+  <si>
+    <t>Browse sanitaryware &amp; bathroom fittings at Alex &amp; Arms Ceramica in Chennai. Explore practical options across sizes, materials, and designs.</t>
+  </si>
+  <si>
+    <t>Sanitaryware &amp; Bathroom Fittings in Chennai | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/sanitaryware-bathroom-fittings</t>
+  </si>
+  <si>
+    <t>Explore sanitaryware and bathroom fitting options that balance utility, comfort, and modern design.</t>
+  </si>
+  <si>
+    <t>western toilet price chennai</t>
+  </si>
+  <si>
+    <t>grohe wall hung toilet price, grohe wc price, handicap toilet accessories near me, hindware automatic toilet price, hindware bathroom indian toilet</t>
+  </si>
+  <si>
+    <t>Browse toilets and water closets at Alex &amp; Arms Ceramica in Chennai. Explore practical options across sizes, materials, and designs.</t>
+  </si>
+  <si>
+    <t>Toilets and Water Closets | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/sanitaryware-bathroom-fittings/toilets-water-closets</t>
+  </si>
+  <si>
+    <t>Browse toilet and water closet options across layouts and styles for homes and shared spaces.</t>
+  </si>
+  <si>
+    <t>urinal price chennai</t>
+  </si>
+  <si>
+    <t>bathroom urinal price, hindware urinal basin price, hindware urinal pot price, hindware urinal price, ladies urinal hindware price, mens urinal price</t>
+  </si>
+  <si>
+    <t>Browse urinals at Alex &amp; Arms Ceramica in Chennai. Explore practical options across sizes, materials, and designs.</t>
+  </si>
+  <si>
+    <t>Urinals | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/sanitaryware-bathroom-fittings/urinals</t>
+  </si>
+  <si>
+    <t>Find urinal options designed for efficient use, easy cleaning, and dependable performance.</t>
+  </si>
+  <si>
+    <t>wash basin chennai</t>
+  </si>
+  <si>
+    <t>designer wash basin chennai, designer wash basin in chennai, grohe wash basin price, hindware toilet basin price, rak basin price, rak ceramics basin price</t>
+  </si>
+  <si>
+    <t>Browse wash basins at Alex &amp; Arms Ceramica in Chennai. Explore practical options across sizes, materials, and designs.</t>
+  </si>
+  <si>
+    <t>Wash Basins | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/sanitaryware-bathroom-fittings/wash-basins</t>
+  </si>
+  <si>
+    <t>Explore wash basin options in a range of designs for bathrooms and wash areas.</t>
+  </si>
+  <si>
+    <t>bathroom taps chennai</t>
+  </si>
+  <si>
+    <t>ao smith faucet, commercial lavatory faucet, franke sinks and faucets, grohe automatic faucet, grohe bathroom faucets, grohe bathroom sink faucets, grohe bathtub faucet, grohe concetto faucet</t>
+  </si>
+  <si>
+    <t>Browse taps &amp; faucets at Alex &amp; Arms Ceramica in Chennai. Explore practical options across sizes, materials, and designs.</t>
+  </si>
+  <si>
+    <t>Taps &amp; Faucets | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/sanitaryware-bathroom-fittings/taps-faucets</t>
+  </si>
+  <si>
+    <t>Compare taps and faucet options for bathrooms and kitchens, from basic utility to premium designs.</t>
+  </si>
+  <si>
+    <t>bathtub chennai</t>
+  </si>
+  <si>
+    <t>bathtub rooms in chennai, hindware bathtub price in chennai, jacuzzi bath in chennai</t>
+  </si>
+  <si>
+    <t>Browse bath &amp; wellness at Alex &amp; Arms Ceramica in Chennai. Explore practical options across sizes, materials, and designs.</t>
+  </si>
+  <si>
+    <t>Bath &amp; Wellness | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/sanitaryware-bathroom-fittings/bath-wellness</t>
+  </si>
+  <si>
+    <t>Explore bathtubs, enclosures, and wellness products designed for comfort and everyday use.</t>
+  </si>
+  <si>
+    <t>bathroom accessories chennai</t>
+  </si>
+  <si>
+    <t>bathroom accessories disabled persons, bathroom accessories shop in chennai, disabled bathroom accessories, grohe bathroom accessories, grohe essentials towel ring, grohe towel ring, handicap bathroom accessories, public bathroom accessories</t>
+  </si>
+  <si>
+    <t>Browse bathroom accessories at Alex &amp; Arms Ceramica in Chennai. Explore practical options across sizes, materials, and designs.</t>
+  </si>
+  <si>
+    <t>Bathroom Accessories | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/sanitaryware-bathroom-fittings/bathroom-accessories</t>
+  </si>
+  <si>
+    <t>Browse bathroom accessories that improve daily convenience while matching your overall design style.</t>
+  </si>
+  <si>
+    <t>bathroom mirrors chennai</t>
+  </si>
+  <si>
+    <t>bathroom mirror shop near me, bathroom cabinets chennai, bathroom mirror cabinet chennai, bathroom mirror low price, bathroom mirror price, bathroom mirror stores near me, bathroom mirrors for sale near me, bathroom mirrors near me</t>
+  </si>
+  <si>
+    <t>Browse mirrors &amp; cabinets at Alex &amp; Arms Ceramica in Chennai. Explore practical options across sizes, materials, and designs.</t>
+  </si>
+  <si>
+    <t>Mirrors &amp; Cabinets | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/sanitaryware-bathroom-fittings/mirrors-cabinets</t>
+  </si>
+  <si>
+    <t>Find mirrors and cabinets that combine practical storage with stylish bathroom design.</t>
+  </si>
+  <si>
+    <t>water heater chennai</t>
+  </si>
+  <si>
+    <t>ao smith geyser, geyser chennai price, bathroom water heaters</t>
+  </si>
+  <si>
+    <t>Explore instant, storage, and energy-efficient water heater options from trusted brands for everyday hot water needs in Chennai.</t>
+  </si>
+  <si>
+    <t>Water Heaters | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/sanitaryware-bathroom-fittings/water-heaters</t>
+  </si>
+  <si>
+    <t>Explore water heater options for different usage patterns, capacities, and energy preferences.</t>
+  </si>
+  <si>
+    <t>floor drain chennai</t>
+  </si>
+  <si>
+    <t>bathroom drain, shower drain, linear drain</t>
+  </si>
+  <si>
+    <t>Explore durable floor drain options for bathrooms, utility areas, and commercial spaces at Alex &amp; Arms Ceramica in Chennai.</t>
+  </si>
+  <si>
+    <t>Floor Drains | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/sanitaryware-bathroom-fittings/floor-drains</t>
+  </si>
+  <si>
+    <t>Browse floor drain options built for reliable water flow, safety, and practical installation.</t>
+  </si>
+  <si>
+    <t>accessible bathroom products chennai</t>
+  </si>
+  <si>
+    <t>accessible bathroom shower, accessories for disabled bathroom, accessories for handicapped bathrooms, bath aids for disabled</t>
+  </si>
+  <si>
+    <t>Explore accessibility-focused bathroom solutions designed for comfort, safety, and ease of use at Alex &amp; Arms Ceramica in Chennai.</t>
+  </si>
+  <si>
+    <t>Differently-Abled Bath Products | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/sanitaryware-bathroom-fittings/differently-abled-bath-products</t>
+  </si>
+  <si>
+    <t>Explore accessibility-focused bathroom products designed to improve safety and ease of movement.</t>
+  </si>
+  <si>
+    <t>commercial restroom solutions chennai</t>
+  </si>
+  <si>
+    <t>commercial restroom, commercial restroom mirrors, commercial restroom partitions, commercial restroom products, commercial restroom sinks, commercial restroom stalls, commercial restroom trash can, commercial toilet partitions</t>
+  </si>
+  <si>
+    <t>Need a page or just card?</t>
+  </si>
+  <si>
+    <t>Explore durable, easy-maintenance solutions for high-traffic commercial restroom spaces at Alex &amp; Arms Ceramica in Chennai.</t>
+  </si>
+  <si>
+    <t>Public Restroom Solutions | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/sanitaryware-bathroom-fittings/public-restroom-solutions</t>
+  </si>
+  <si>
+    <t>Discover durable restroom solutions for high-traffic shared spaces and commercial environments.</t>
+  </si>
+  <si>
+    <t>kitchen appliances and sinks chennai</t>
+  </si>
+  <si>
+    <t>carysil kitchen sink, franke kitchen sink, kitchen sink chennai, best kitchen chimney in chennai, carysil kitchen sink dealers near me, carysil kitchen sink near me, carysil kitchen sink price</t>
+  </si>
+  <si>
+    <t>Browse kitchen appliances &amp; sinks at Alex &amp; Arms Ceramica in Chennai. Explore practical options across sizes, materials, and designs.</t>
+  </si>
+  <si>
+    <t>Kitchen Appliances &amp; Sinks in Chennai | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/kitchen-appliances-sinks</t>
+  </si>
+  <si>
+    <t>Explore sinks and kitchen essentials designed for practical everyday cooking and easy upkeep.</t>
+  </si>
+  <si>
+    <t>kitchen sink chennai</t>
+  </si>
+  <si>
+    <t>carysil kitchen sink dealers near me, carysil kitchen sink near me, carysil kitchen sink price, carysil quartz sink price, carysil stainless steel sink price, franke kitchen sink chennai, franke kitchen sink near me, franke kitchen sink price</t>
+  </si>
+  <si>
+    <t>Browse sinks at Alex &amp; Arms Ceramica in Chennai. Explore practical options across sizes, materials, and designs.</t>
+  </si>
+  <si>
+    <t>Sinks | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/kitchen-appliances-sinks/sinks</t>
+  </si>
+  <si>
+    <t>Explore essential kitchen appliances and sinks for practical kitchen planning.</t>
+  </si>
+  <si>
+    <t>kitchen chimney chennai</t>
+  </si>
+  <si>
+    <t>best kitchen chimney in chennai, carysil chimney price, chimney price chennai, chimney price in chennai, chimney showroom chennai, chimney showroom in chennai, electric chimney price in chennai</t>
+  </si>
+  <si>
+    <t>Explore kitchen chimney options designed for cleaner cooking and everyday convenience at Alex &amp; Arms Ceramica in Chennai.</t>
+  </si>
+  <si>
+    <t>Chimneys | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/kitchen-appliances-sinks/chimneys</t>
+  </si>
+  <si>
+    <t>Find chimney options that help manage smoke and odors for cleaner, more comfortable kitchens.</t>
+  </si>
+  <si>
+    <t>kitchen sink faucets chennai</t>
+  </si>
+  <si>
+    <t>kitchen sink chennai, carysil kitchen sink dealers near me, carysil kitchen sink near me, carysil kitchen sink price, franke kitchen sink chennai, franke kitchen sink near me, franke kitchen sink price, hindware kitchen sink dealers near me</t>
+  </si>
+  <si>
+    <t>Browse kitchen sinks &amp; faucets at Alex &amp; Arms Ceramica in Chennai. Explore practical options across sizes, materials, and designs.</t>
+  </si>
+  <si>
+    <t>Kitchen Sinks &amp; Faucets | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/kitchen-appliances-sinks/kitchen-sinks-faucets</t>
+  </si>
+  <si>
+    <t>Browse coordinated kitchen sink and faucet options for functionality, fit, and finish.</t>
+  </si>
+  <si>
+    <t>Placeholder</t>
+  </si>
+  <si>
+    <t>kitchen appliances chennai</t>
+  </si>
+  <si>
+    <t>carysil kitchen appliances, hoods and hobs chennai</t>
+  </si>
+  <si>
+    <t>Need to confirm if needed</t>
+  </si>
+  <si>
+    <t>Explore practical kitchen appliance options for modern, efficient daily use at Alex &amp; Arms Ceramica in Chennai.</t>
+  </si>
+  <si>
+    <t>Other Appliances | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/products/kitchen-appliances-sinks/other-appliances</t>
+  </si>
+  <si>
+    <t>Explore practical appliance options that complement your kitchen setup and daily routine.</t>
+  </si>
+  <si>
+    <t>grohe chennai</t>
+  </si>
+  <si>
+    <t>grohe dealers, grohe dealers in chennai, grohe health faucet price, grohe price grohe shop, grohe shop online, grohe shower price</t>
+  </si>
+  <si>
+    <t>Browse our collection of GROHE products at Alex &amp; Arms Ceramica in Chennai. Explore premium fittings for modern bathroom and kitchen spaces.</t>
+  </si>
+  <si>
+    <t>GROHE Dealer in Chennai | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/brands/grohe</t>
+  </si>
+  <si>
+    <t>GROHE at Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>Browse GROHE categories available at our Chennai showroom and shortlist options for your space.</t>
+  </si>
+  <si>
+    <t>rak ceramics chennai</t>
+  </si>
+  <si>
+    <t>price of rak tiles, rak basin price, rak ceramic dealers, rak ceramic near me, rak ceramic tiles price, rak ceramics basin price, rak ceramics dealers in chennai, rak ceramics dealers near me</t>
+  </si>
+  <si>
+    <t>Browse our collection of RAK Ceramics products at Alex &amp; Arms Ceramica in Chennai. Explore quality tiles and sanitaryware for modern spaces.</t>
+  </si>
+  <si>
+    <t>RAK Ceramics Dealer in Chennai | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/brands/rak-ceramics</t>
+  </si>
+  <si>
+    <t>RAK Ceramics at Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>Explore RAK Ceramics categories in-store and find practical options for tile and sanitaryware needs.</t>
+  </si>
+  <si>
+    <t>agl bathroom tiles price</t>
+  </si>
+  <si>
+    <t>agl cool roof tiles price, agl dealers, agl dealers near me, agl double charge vitrified tiles price, agl floor tiles price, agl parking tiles price, agl quartz dealers near me, agl tile adhesive price</t>
+  </si>
+  <si>
+    <t>Browse our collection of AGL products at Alex &amp; Arms Ceramica in Chennai. Explore stylish tiles and surface solutions for home and commercial spaces.</t>
+  </si>
+  <si>
+    <t>AGL Dealer in Chennai | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/brands/agl</t>
+  </si>
+  <si>
+    <t>AGL at Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>Browse AGL tile and surface categories suited to both design-focused and utility-led spaces.</t>
+  </si>
+  <si>
+    <t>hindware showroom near me</t>
+  </si>
+  <si>
+    <t>flush tank hindware price, hindware authorised dealer near me, hindware automatic toilet price, hindware basic commode price, hindware bathroom hindware indian toilet seat price, hindware bathtub price in chennai, hindware cascade commode price, hindware ceramic flush tank price</t>
+  </si>
+  <si>
+    <t>Browse our collection of Hindware products at Alex &amp; Arms Ceramica in Chennai. Explore sanitaryware, faucets, and bathroom essentials.</t>
+  </si>
+  <si>
+    <t>Hindware Dealer in Chennai | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/brands/hindware</t>
+  </si>
+  <si>
+    <t>Hindware at Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>Explore Hindware products at our Chennai showroom, including sanitaryware, faucets, and bathroom essentials for your space needs.</t>
+  </si>
+  <si>
+    <t>carysil chennai</t>
+  </si>
+  <si>
+    <t>carysil chimney price, carysil dealers in chennai, carysil dealers near me, carysil double bowl sink price, carysil food waste disposer price, carysil granite sink price, carysil kitchen sink dealers near me, carysil kitchen sink near me</t>
+  </si>
+  <si>
+    <t>Browse our collection of Carysil products at Alex &amp; Arms Ceramica in Chennai. Explore kitchen sinks and appliances for practical modern kitchens.</t>
+  </si>
+  <si>
+    <t>Carysil Dealer in Chennai | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/brands/carysil</t>
+  </si>
+  <si>
+    <t>Carysil at Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>Browse Carysil kitchen-focused categories, including sinks and related solutions for modern homes.</t>
+  </si>
+  <si>
+    <t>best price franke sinks</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> franke double sink price, franke kitchen sink chennai, franke kitchen sink near me, franke kitchen sink price, franke sink dealers in chennai, franke sink price, franke sinks near me</t>
+  </si>
+  <si>
+    <t>Browse our collection of Franke products at Alex &amp; Arms Ceramica in Chennai. Explore premium kitchen sinks and solutions for modern kitchens.</t>
+  </si>
+  <si>
+    <t>Franke Dealer in Chennai | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/brands/franke</t>
+  </si>
+  <si>
+    <t>Franke at Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>Explore Franke sink and kitchen categories with premium options for durable everyday use.</t>
+  </si>
+  <si>
+    <t>pidilite roff price</t>
+  </si>
+  <si>
+    <t>pidilite roff tile adhesive price, roff adhesive price, roff cement for tiles price, roff cement near me</t>
+  </si>
+  <si>
+    <t>Browse our collection of Roff products at Alex &amp; Arms Ceramica in Chennai. Explore tile adhesives and installation solutions for reliable finishing.</t>
+  </si>
+  <si>
+    <t>Roff Dealer in Chennai | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/brands/roff</t>
+  </si>
+  <si>
+    <t>Roff at Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>Browse Roff installation categories, including adhesives and support materials for tile work.</t>
+  </si>
+  <si>
+    <t>ardex endura chennai</t>
+  </si>
+  <si>
+    <t>ardex endura, ardex dealer, ardex endura dealers near me, ardex endura diamond star price, ardex endura epoxy grout price, ardex endura gold star price, ardex endura price, ardex near me</t>
+  </si>
+  <si>
+    <t>Browse our collection of Ardex Endura products at Alex &amp; Arms Ceramica in Chennai. Explore adhesives, grouts, and installation materials.</t>
+  </si>
+  <si>
+    <t>Ardex Endura Dealer in Chennai | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/brands/ardex-endura</t>
+  </si>
+  <si>
+    <t>Ardex Endura at Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>Explore Ardex Endura categories for installation, grouting, and finishing requirements.</t>
+  </si>
+  <si>
+    <t>ao smith authorized dealers</t>
+  </si>
+  <si>
+    <t>ao smith booster pump price, ao smith chennai, ao smith dealers, ao smith geyser chennai, ao smith water heater</t>
+  </si>
+  <si>
+    <t>Browse our collection of AO Smith products at Alex &amp; Arms Ceramica in Chennai. Explore water heaters and home comfort solutions for daily use.</t>
+  </si>
+  <si>
+    <t>AO Smith Dealer in Chennai | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/brands/ao-smith</t>
+  </si>
+  <si>
+    <t>AO Smith at Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>Browse AO Smith categories focused on hot water comfort and related home solutions.</t>
+  </si>
+  <si>
+    <t>gas geyser racold price</t>
+  </si>
+  <si>
+    <t>price of racold solar water heater, racold litre water heater, geyser litre</t>
+  </si>
+  <si>
+    <t>Browse our collection of Racold products at Alex &amp; Arms Ceramica in Chennai. Explore water heaters and geyser solutions for everyday needs.</t>
+  </si>
+  <si>
+    <t>Racold Dealer in Chennai | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/brands/racold</t>
+  </si>
+  <si>
+    <t>Racold at Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>Explore Racold water heating categories for household and everyday space requirements.</t>
+  </si>
+  <si>
+    <t>bathroom solutions chennai</t>
+  </si>
+  <si>
+    <t>bathroom accessories chennai, bathroom fittings chennai, bathroom fittings wholesale in chennai, bathroom accessories shop in chennai, bathroom fittings showroom in chennai, bathtub chennai</t>
+  </si>
+  <si>
+    <t>Discover bathroom solutions at Alex &amp; Arms Ceramica in Chennai, including tiles, sanitaryware, faucets, and accessories for modern spaces.</t>
+  </si>
+  <si>
+    <t>Bathroom Solutions | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/bathroom-solutions</t>
+  </si>
+  <si>
+    <t>Discover coordinated bathroom options across sanitaryware, faucets, accessories, and related categories.</t>
+  </si>
+  <si>
+    <t>kitchen essentials chennai</t>
+  </si>
+  <si>
+    <t>kitchen sink chennai, best kitchen chimney in chennai, carysil kitchen sink dealers near me, carysil kitchen sink near me, carysil kitchen sink price, franke kitchen sink chennai, franke kitchen sink near me</t>
+  </si>
+  <si>
+    <t>Discover kitchen essentials at Alex &amp; Arms Ceramica in Chennai, including sinks, faucets, chimneys, and appliances for practical kitchens.</t>
+  </si>
+  <si>
+    <t>Kitchen Essentials | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/kitchen-essentials</t>
+  </si>
+  <si>
+    <t>Discover practical kitchen options across sinks, faucets, chimneys, and everyday appliances.</t>
+  </si>
+  <si>
+    <t>parking tiles chennai</t>
+  </si>
+  <si>
+    <t>agl parking tiles, agl parking tiles price, car parking tiles chennai, car parking tiles in chennai, car parking tiles price in chennai, parking tiles price in chennai, rak ceramics parking tiles, rak outdoor tiles</t>
+  </si>
+  <si>
+    <t>Discover outdoor and parking solutions at Alex &amp; Arms Ceramica in Chennai, including durable tiles and practical surface options for exterior areas.</t>
+  </si>
+  <si>
+    <t>Outdoor &amp; Parking | Alex &amp; Arms Ceramica</t>
+  </si>
+  <si>
+    <t>/outdoor-parking</t>
+  </si>
+  <si>
+    <t>Discover durable outdoor and parking surface options designed for daily use and long-term performance.</t>
+  </si>
+  <si>
+    <t>Collections</t>
+  </si>
+  <si>
+    <t>Collections Landing page</t>
+  </si>
+  <si>
+    <t>tiles collections chennai</t>
+  </si>
+  <si>
+    <t>Featured Collections</t>
+  </si>
+  <si>
+    <t>Browse curated collections from leading brands, including tile and product ranges for bathrooms, kitchens, and more.</t>
+  </si>
   <si>
     <t>Level 1 (Main Category)</t>
   </si>
@@ -37,12 +952,6 @@
     <t>Level 3 (Cards to dispay on L2 page)</t>
   </si>
   <si>
-    <t>Tiles</t>
-  </si>
-  <si>
-    <t>Vitrified Tiles</t>
-  </si>
-  <si>
     <t>Vitrified Wall Tiles</t>
   </si>
   <si>
@@ -70,9 +979,6 @@
     <t>&gt; Product/product list</t>
   </si>
   <si>
-    <t>Ceramic Tiles</t>
-  </si>
-  <si>
     <t>Ceramic Wall Tiles</t>
   </si>
   <si>
@@ -91,21 +997,9 @@
     <t>Designer Tiles (Subway, Geometric, Hexa?)</t>
   </si>
   <si>
-    <t>Wall Tiles</t>
-  </si>
-  <si>
     <t>[TBD]</t>
   </si>
   <si>
-    <t>Floor Tiles</t>
-  </si>
-  <si>
-    <t>Sanitaryware &amp; Bathroom Fittings</t>
-  </si>
-  <si>
-    <t>Toilets and Water Closets</t>
-  </si>
-  <si>
     <t>One Piece</t>
   </si>
   <si>
@@ -127,12 +1021,6 @@
     <t>Indian Closets</t>
   </si>
   <si>
-    <t>Urinals</t>
-  </si>
-  <si>
-    <t>Wash Basins</t>
-  </si>
-  <si>
     <t>Countertop Basins</t>
   </si>
   <si>
@@ -148,9 +1036,6 @@
     <t>Integrated Vanities</t>
   </si>
   <si>
-    <t>Taps &amp; Faucets</t>
-  </si>
-  <si>
     <t>Pillar Cocks &amp; Bib Cock</t>
   </si>
   <si>
@@ -181,9 +1066,6 @@
     <t>Designer Taps &amp; Showers</t>
   </si>
   <si>
-    <t>Bath &amp; Wellness</t>
-  </si>
-  <si>
     <t>Bathtubs</t>
   </si>
   <si>
@@ -196,9 +1078,6 @@
     <t>Shower Panels</t>
   </si>
   <si>
-    <t>Bathroom Accessories</t>
-  </si>
-  <si>
     <t>Towel Rails and Ring</t>
   </si>
   <si>
@@ -217,9 +1096,6 @@
     <t>Designer Bath Accessories</t>
   </si>
   <si>
-    <t>Mirrors &amp; Cabinets</t>
-  </si>
-  <si>
     <t>Mirrors</t>
   </si>
   <si>
@@ -232,9 +1108,6 @@
     <t>Designer</t>
   </si>
   <si>
-    <t>Water Heaters</t>
-  </si>
-  <si>
     <t>Instant</t>
   </si>
   <si>
@@ -247,21 +1120,6 @@
     <t>Heat Pumps</t>
   </si>
   <si>
-    <t>Floor Drains</t>
-  </si>
-  <si>
-    <t>Differently-Abled Bath Products</t>
-  </si>
-  <si>
-    <t>Public Restroom Solutions</t>
-  </si>
-  <si>
-    <t>Kitchen Appliances &amp; Sinks</t>
-  </si>
-  <si>
-    <t>Sinks</t>
-  </si>
-  <si>
     <t>Stainless Steel Sinks</t>
   </si>
   <si>
@@ -271,15 +1129,6 @@
     <t>Ceramic Sinks</t>
   </si>
   <si>
-    <t>Chimneys</t>
-  </si>
-  <si>
-    <t>Kitchen Sinks &amp; Faucets</t>
-  </si>
-  <si>
-    <t>Other Appliances</t>
-  </si>
-  <si>
     <t>TBD based on volume</t>
   </si>
   <si>
@@ -292,45 +1141,9 @@
     <t>Plumber</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>GROHE</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>RAK Ceramics</t>
-  </si>
-  <si>
-    <t>AGL</t>
-  </si>
-  <si>
     <t>Crystal Ceramics</t>
   </si>
   <si>
-    <t>Hindware</t>
-  </si>
-  <si>
-    <t>Carysil</t>
-  </si>
-  <si>
-    <t>Franke</t>
-  </si>
-  <si>
-    <t>Roff</t>
-  </si>
-  <si>
-    <t>Ardex Endura</t>
-  </si>
-  <si>
-    <t>AO Smith</t>
-  </si>
-  <si>
-    <t>Racold</t>
-  </si>
-  <si>
     <t>Watertec</t>
   </si>
   <si>
@@ -355,19 +1168,13 @@
     <t>Name for title</t>
   </si>
   <si>
-    <t>Room</t>
-  </si>
-  <si>
     <t>Associated L2 or L3 cards</t>
   </si>
   <si>
-    <t>Bathroom Solutions</t>
-  </si>
-  <si>
     <t>Bathroom</t>
   </si>
   <si>
-    <t>Toilets and Water Closets, Wash Basins, Urinals, Taps &amp; Faucets, Bath &amp; Wellness, Bathroom Accessories, Mirrors &amp; Cabinets, Water Heaters, Floor Drains</t>
+    <t>Toilets and Water Closets, Wash Basins, Urinals, Taps &amp; Faucets, Bath &amp; Wellness, Bathroom Accessories, Mirrors &amp; Cabinets, Water Heaters, Floor Drains, Differently-Abled Bath Products</t>
   </si>
   <si>
     <t>Kitchen</t>
@@ -382,47 +1189,77 @@
     <t>Parking (outdoor tiles), Floor Tiles, Wall Tiles, Floor Drains</t>
   </si>
   <si>
-    <t>Utility Solutions</t>
-  </si>
-  <si>
-    <t>Utility</t>
-  </si>
-  <si>
-    <t>Water Heaters, Sinks, Floor Drains, Other Appliances</t>
-  </si>
-  <si>
     <t>Commercial Restroom Solutions</t>
   </si>
   <si>
     <t>Public Restroom Solutions, Differently-Abled Bath Products, Urinals, Toilets and Water Closets, Floor Drains, Taps &amp; Faucets</t>
   </si>
   <si>
-    <t>Home</t>
+    <t>Nav Items</t>
+  </si>
+  <si>
+    <t>Home page</t>
   </si>
   <si>
     <t>Products</t>
   </si>
   <si>
+    <t>Product Category Taxonomy</t>
+  </si>
+  <si>
     <t>Browse by Room</t>
   </si>
   <si>
     <t>Contact</t>
   </si>
   <si>
-    <t>Nav Items</t>
-  </si>
-  <si>
-    <t>Home page</t>
-  </si>
-  <si>
-    <t>Product Category Taxonomy</t>
+    <t>Hero banner</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>CTA</t>
+  </si>
+  <si>
+    <t>Short Intro</t>
+  </si>
+  <si>
+    <t>Showroom Experience</t>
+  </si>
+  <si>
+    <t>Our Showroom</t>
+  </si>
+  <si>
+    <t>Map section</t>
+  </si>
+  <si>
+    <t>Footer</t>
+  </si>
+  <si>
+    <t>Gallery</t>
+  </si>
+  <si>
+    <t>Visit Our Vadapalani Showroom</t>
+  </si>
+  <si>
+    <t>Highlights</t>
+  </si>
+  <si>
+    <t>Section Name</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Details</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,8 +1282,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,6 +1325,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -495,7 +1344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -515,8 +1364,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -819,11 +1672,1840 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N102"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" customWidth="1"/>
+    <col min="10" max="10" width="19.1640625" customWidth="1"/>
+    <col min="11" max="11" width="39.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="14"/>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" s="12"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9" t="s">
+        <v>80</v>
+      </c>
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I10" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H11" t="s">
+        <v>116</v>
+      </c>
+      <c r="I11" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" t="s">
+        <v>122</v>
+      </c>
+      <c r="I12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" t="s">
+        <v>127</v>
+      </c>
+      <c r="H13" t="s">
+        <v>128</v>
+      </c>
+      <c r="I13" t="s">
+        <v>80</v>
+      </c>
+      <c r="J13" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" t="s">
+        <v>132</v>
+      </c>
+      <c r="G14" t="s">
+        <v>133</v>
+      </c>
+      <c r="H14" t="s">
+        <v>134</v>
+      </c>
+      <c r="I14" t="s">
+        <v>80</v>
+      </c>
+      <c r="J14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D15" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" t="s">
+        <v>138</v>
+      </c>
+      <c r="G15" t="s">
+        <v>139</v>
+      </c>
+      <c r="H15" t="s">
+        <v>140</v>
+      </c>
+      <c r="I15" t="s">
+        <v>80</v>
+      </c>
+      <c r="J15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" t="s">
+        <v>144</v>
+      </c>
+      <c r="G16" t="s">
+        <v>145</v>
+      </c>
+      <c r="H16" t="s">
+        <v>146</v>
+      </c>
+      <c r="I16" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" t="s">
+        <v>150</v>
+      </c>
+      <c r="G17" t="s">
+        <v>151</v>
+      </c>
+      <c r="H17" t="s">
+        <v>152</v>
+      </c>
+      <c r="I17" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" t="s">
+        <v>155</v>
+      </c>
+      <c r="E18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" t="s">
+        <v>156</v>
+      </c>
+      <c r="G18" t="s">
+        <v>157</v>
+      </c>
+      <c r="H18" t="s">
+        <v>158</v>
+      </c>
+      <c r="I18" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>160</v>
+      </c>
+      <c r="D19" t="s">
+        <v>161</v>
+      </c>
+      <c r="E19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" t="s">
+        <v>162</v>
+      </c>
+      <c r="G19" t="s">
+        <v>163</v>
+      </c>
+      <c r="H19" t="s">
+        <v>164</v>
+      </c>
+      <c r="I19" t="s">
+        <v>80</v>
+      </c>
+      <c r="J19" t="s">
+        <v>26</v>
+      </c>
+      <c r="K19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>166</v>
+      </c>
+      <c r="D20" t="s">
+        <v>167</v>
+      </c>
+      <c r="E20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" t="s">
+        <v>168</v>
+      </c>
+      <c r="G20" t="s">
+        <v>169</v>
+      </c>
+      <c r="H20" t="s">
+        <v>170</v>
+      </c>
+      <c r="I20" t="s">
+        <v>80</v>
+      </c>
+      <c r="J20" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F21" t="s">
+        <v>175</v>
+      </c>
+      <c r="G21" t="s">
+        <v>176</v>
+      </c>
+      <c r="H21" t="s">
+        <v>177</v>
+      </c>
+      <c r="I21" t="s">
+        <v>65</v>
+      </c>
+      <c r="J21" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>179</v>
+      </c>
+      <c r="D22" t="s">
+        <v>180</v>
+      </c>
+      <c r="E22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" t="s">
+        <v>181</v>
+      </c>
+      <c r="G22" t="s">
+        <v>182</v>
+      </c>
+      <c r="H22" t="s">
+        <v>183</v>
+      </c>
+      <c r="I22" t="s">
+        <v>80</v>
+      </c>
+      <c r="J22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>185</v>
+      </c>
+      <c r="D23" t="s">
+        <v>186</v>
+      </c>
+      <c r="E23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" t="s">
+        <v>187</v>
+      </c>
+      <c r="G23" t="s">
+        <v>188</v>
+      </c>
+      <c r="H23" t="s">
+        <v>189</v>
+      </c>
+      <c r="I23" t="s">
+        <v>80</v>
+      </c>
+      <c r="J23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K23" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>191</v>
+      </c>
+      <c r="D24" t="s">
+        <v>192</v>
+      </c>
+      <c r="E24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" t="s">
+        <v>193</v>
+      </c>
+      <c r="G24" t="s">
+        <v>194</v>
+      </c>
+      <c r="H24" t="s">
+        <v>195</v>
+      </c>
+      <c r="I24" t="s">
+        <v>80</v>
+      </c>
+      <c r="J24" t="s">
+        <v>31</v>
+      </c>
+      <c r="K24" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>197</v>
+      </c>
+      <c r="D25" t="s">
+        <v>198</v>
+      </c>
+      <c r="E25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" t="s">
+        <v>199</v>
+      </c>
+      <c r="G25" t="s">
+        <v>200</v>
+      </c>
+      <c r="H25" t="s">
+        <v>201</v>
+      </c>
+      <c r="I25" t="s">
+        <v>80</v>
+      </c>
+      <c r="J25" t="s">
+        <v>32</v>
+      </c>
+      <c r="K25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="F26" t="s">
+        <v>207</v>
+      </c>
+      <c r="G26" t="s">
+        <v>208</v>
+      </c>
+      <c r="H26" t="s">
+        <v>209</v>
+      </c>
+      <c r="I26" t="s">
+        <v>65</v>
+      </c>
+      <c r="J26" t="s">
+        <v>33</v>
+      </c>
+      <c r="K26" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>211</v>
+      </c>
+      <c r="D27" t="s">
+        <v>212</v>
+      </c>
+      <c r="E27" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" t="s">
+        <v>213</v>
+      </c>
+      <c r="G27" t="s">
+        <v>214</v>
+      </c>
+      <c r="H27" t="s">
+        <v>215</v>
+      </c>
+      <c r="I27" t="s">
+        <v>65</v>
+      </c>
+      <c r="J27" t="s">
+        <v>216</v>
+      </c>
+      <c r="K27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s">
+        <v>218</v>
+      </c>
+      <c r="D28" t="s">
+        <v>219</v>
+      </c>
+      <c r="E28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" t="s">
+        <v>220</v>
+      </c>
+      <c r="G28" t="s">
+        <v>221</v>
+      </c>
+      <c r="H28" t="s">
+        <v>222</v>
+      </c>
+      <c r="I28" t="s">
+        <v>65</v>
+      </c>
+      <c r="J28" t="s">
+        <v>223</v>
+      </c>
+      <c r="K28" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D29" t="s">
+        <v>226</v>
+      </c>
+      <c r="E29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" t="s">
+        <v>227</v>
+      </c>
+      <c r="G29" t="s">
+        <v>228</v>
+      </c>
+      <c r="H29" t="s">
+        <v>229</v>
+      </c>
+      <c r="I29" t="s">
+        <v>65</v>
+      </c>
+      <c r="J29" t="s">
+        <v>230</v>
+      </c>
+      <c r="K29" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>232</v>
+      </c>
+      <c r="D30" t="s">
+        <v>233</v>
+      </c>
+      <c r="E30" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" t="s">
+        <v>234</v>
+      </c>
+      <c r="G30" t="s">
+        <v>235</v>
+      </c>
+      <c r="H30" t="s">
+        <v>236</v>
+      </c>
+      <c r="I30" t="s">
+        <v>65</v>
+      </c>
+      <c r="J30" t="s">
+        <v>237</v>
+      </c>
+      <c r="K30" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>239</v>
+      </c>
+      <c r="D31" t="s">
+        <v>240</v>
+      </c>
+      <c r="E31" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" t="s">
+        <v>241</v>
+      </c>
+      <c r="G31" t="s">
+        <v>242</v>
+      </c>
+      <c r="H31" t="s">
+        <v>243</v>
+      </c>
+      <c r="I31" t="s">
+        <v>65</v>
+      </c>
+      <c r="J31" t="s">
+        <v>244</v>
+      </c>
+      <c r="K31" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>246</v>
+      </c>
+      <c r="D32" t="s">
+        <v>247</v>
+      </c>
+      <c r="E32" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" t="s">
+        <v>248</v>
+      </c>
+      <c r="G32" t="s">
+        <v>249</v>
+      </c>
+      <c r="H32" t="s">
+        <v>250</v>
+      </c>
+      <c r="I32" t="s">
+        <v>65</v>
+      </c>
+      <c r="J32" t="s">
+        <v>251</v>
+      </c>
+      <c r="K32" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" t="s">
+        <v>253</v>
+      </c>
+      <c r="D33" t="s">
+        <v>254</v>
+      </c>
+      <c r="E33" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" t="s">
+        <v>255</v>
+      </c>
+      <c r="G33" t="s">
+        <v>256</v>
+      </c>
+      <c r="H33" t="s">
+        <v>257</v>
+      </c>
+      <c r="I33" t="s">
+        <v>65</v>
+      </c>
+      <c r="J33" t="s">
+        <v>258</v>
+      </c>
+      <c r="K33" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" t="s">
+        <v>260</v>
+      </c>
+      <c r="D34" t="s">
+        <v>261</v>
+      </c>
+      <c r="E34" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" t="s">
+        <v>262</v>
+      </c>
+      <c r="G34" t="s">
+        <v>263</v>
+      </c>
+      <c r="H34" t="s">
+        <v>264</v>
+      </c>
+      <c r="I34" t="s">
+        <v>65</v>
+      </c>
+      <c r="J34" t="s">
+        <v>265</v>
+      </c>
+      <c r="K34" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s">
+        <v>267</v>
+      </c>
+      <c r="D35" t="s">
+        <v>268</v>
+      </c>
+      <c r="E35" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" t="s">
+        <v>269</v>
+      </c>
+      <c r="G35" t="s">
+        <v>270</v>
+      </c>
+      <c r="H35" t="s">
+        <v>271</v>
+      </c>
+      <c r="I35" t="s">
+        <v>65</v>
+      </c>
+      <c r="J35" t="s">
+        <v>272</v>
+      </c>
+      <c r="K35" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" t="s">
+        <v>274</v>
+      </c>
+      <c r="D36" t="s">
+        <v>275</v>
+      </c>
+      <c r="E36" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" t="s">
+        <v>276</v>
+      </c>
+      <c r="G36" t="s">
+        <v>277</v>
+      </c>
+      <c r="H36" t="s">
+        <v>278</v>
+      </c>
+      <c r="I36" t="s">
+        <v>65</v>
+      </c>
+      <c r="J36" t="s">
+        <v>279</v>
+      </c>
+      <c r="K36" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" t="s">
+        <v>281</v>
+      </c>
+      <c r="D37" t="s">
+        <v>282</v>
+      </c>
+      <c r="E37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F37" t="s">
+        <v>283</v>
+      </c>
+      <c r="G37" t="s">
+        <v>284</v>
+      </c>
+      <c r="H37" t="s">
+        <v>285</v>
+      </c>
+      <c r="I37" t="s">
+        <v>80</v>
+      </c>
+      <c r="J37" t="s">
+        <v>46</v>
+      </c>
+      <c r="K37" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" t="s">
+        <v>287</v>
+      </c>
+      <c r="D38" t="s">
+        <v>288</v>
+      </c>
+      <c r="E38" t="s">
+        <v>61</v>
+      </c>
+      <c r="F38" t="s">
+        <v>289</v>
+      </c>
+      <c r="G38" t="s">
+        <v>290</v>
+      </c>
+      <c r="H38" t="s">
+        <v>291</v>
+      </c>
+      <c r="I38" t="s">
+        <v>80</v>
+      </c>
+      <c r="J38" t="s">
+        <v>47</v>
+      </c>
+      <c r="K38" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" t="s">
+        <v>293</v>
+      </c>
+      <c r="D39" t="s">
+        <v>294</v>
+      </c>
+      <c r="E39" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39" t="s">
+        <v>295</v>
+      </c>
+      <c r="G39" t="s">
+        <v>296</v>
+      </c>
+      <c r="H39" t="s">
+        <v>297</v>
+      </c>
+      <c r="I39" t="s">
+        <v>80</v>
+      </c>
+      <c r="J39" t="s">
+        <v>48</v>
+      </c>
+      <c r="K39" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>299</v>
+      </c>
+      <c r="B40" t="s">
+        <v>300</v>
+      </c>
+      <c r="C40" t="s">
+        <v>301</v>
+      </c>
+      <c r="J40" t="s">
+        <v>302</v>
+      </c>
+      <c r="K40" t="s">
+        <v>303</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17B3851A-64B0-D746-B838-A6449A38529C}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>404</v>
+      </c>
+      <c r="B6" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>402</v>
+      </c>
+      <c r="B7" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B8" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:N101"/>
+  <sheetViews>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -846,13 +3528,13 @@
   <sheetData>
     <row r="1" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>304</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>305</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>306</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -868,65 +3550,65 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="6" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="4" t="s">
-        <v>5</v>
+        <v>307</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>7</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="4" t="s">
-        <v>8</v>
+        <v>310</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>9</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="4" t="s">
-        <v>10</v>
+        <v>312</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>11</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="4" t="s">
-        <v>12</v>
+        <v>314</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>13</v>
+        <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -942,49 +3624,49 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="C10" s="4" t="s">
-        <v>15</v>
+        <v>316</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="C11" s="4" t="s">
-        <v>16</v>
+        <v>317</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>17</v>
+        <v>318</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="C12" s="4" t="s">
-        <v>18</v>
+        <v>319</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="C13" s="4" t="s">
-        <v>19</v>
+        <v>320</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="C14" s="4" t="s">
-        <v>20</v>
+        <v>321</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -993,34 +3675,34 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="C17" s="5" t="s">
-        <v>5</v>
+        <v>307</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="C18" s="5" t="s">
-        <v>15</v>
+        <v>316</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="C19" s="5" t="s">
-        <v>22</v>
+        <v>322</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1029,34 +3711,34 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="C22" s="5" t="s">
-        <v>8</v>
+        <v>310</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="C23" s="5" t="s">
-        <v>16</v>
+        <v>317</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="C24" s="5" t="s">
-        <v>22</v>
+        <v>322</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1064,653 +3746,649 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C28" s="4" t="s">
-        <v>26</v>
+        <v>323</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C29" s="4" t="s">
-        <v>27</v>
+        <v>324</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C30" s="4" t="s">
-        <v>28</v>
+        <v>325</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C31" s="4" t="s">
-        <v>29</v>
+        <v>326</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C32" s="4" t="s">
-        <v>30</v>
+        <v>327</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C33" s="4" t="s">
-        <v>31</v>
+        <v>328</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C34" s="4" t="s">
-        <v>32</v>
+        <v>329</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="3" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C39" s="4" t="s">
-        <v>35</v>
+        <v>330</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C40" s="4" t="s">
-        <v>36</v>
+        <v>331</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C41" s="4" t="s">
-        <v>37</v>
+        <v>332</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C42" s="4" t="s">
-        <v>38</v>
+        <v>333</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C43" s="4" t="s">
-        <v>39</v>
+        <v>334</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C46" s="4" t="s">
-        <v>41</v>
+        <v>335</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C47" s="4" t="s">
-        <v>42</v>
+        <v>336</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C48" s="4" t="s">
-        <v>43</v>
+        <v>337</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C49" s="4" t="s">
-        <v>44</v>
+        <v>338</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C50" s="4" t="s">
-        <v>45</v>
+        <v>339</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C51" s="4" t="s">
-        <v>46</v>
+        <v>340</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C52" s="4" t="s">
-        <v>47</v>
+        <v>341</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C53" s="4" t="s">
-        <v>48</v>
+        <v>342</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C54" s="4" t="s">
-        <v>49</v>
+        <v>343</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C55" s="4" t="s">
-        <v>50</v>
+        <v>344</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" s="3" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C58" s="4" t="s">
-        <v>52</v>
+        <v>345</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C59" s="4" t="s">
-        <v>53</v>
+        <v>346</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C60" s="4" t="s">
-        <v>54</v>
+        <v>347</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C61" s="4" t="s">
-        <v>55</v>
+        <v>348</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B63" s="3" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C64" s="4" t="s">
-        <v>57</v>
+        <v>349</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C65" s="4" t="s">
-        <v>58</v>
+        <v>350</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C66" s="4" t="s">
-        <v>59</v>
+        <v>351</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C67" s="4" t="s">
-        <v>60</v>
+        <v>352</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C68" s="4" t="s">
-        <v>61</v>
+        <v>353</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C69" s="4" t="s">
-        <v>62</v>
+        <v>354</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B71" s="3" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C72" s="4" t="s">
-        <v>64</v>
+        <v>355</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C73" s="4" t="s">
-        <v>65</v>
+        <v>356</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C74" s="4" t="s">
-        <v>66</v>
+        <v>357</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C75" s="4" t="s">
-        <v>67</v>
+        <v>358</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B77" s="3" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C78" s="4" t="s">
-        <v>69</v>
+        <v>359</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C79" s="4" t="s">
-        <v>70</v>
+        <v>360</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C80" s="4" t="s">
-        <v>71</v>
+        <v>361</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C81" s="4" t="s">
-        <v>72</v>
+        <v>362</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B83" s="3" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B85" s="3" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="C85" s="8"/>
       <c r="D85" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B87" s="3" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="C87" s="8"/>
       <c r="D87" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="9" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B90" s="3" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C91" s="4" t="s">
-        <v>78</v>
+        <v>363</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C92" s="4" t="s">
-        <v>79</v>
+        <v>364</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C93" s="4" t="s">
-        <v>80</v>
+        <v>365</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B95" s="3" t="s">
-        <v>81</v>
+        <v>31</v>
       </c>
       <c r="C95" s="8"/>
       <c r="D95" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B97" s="3" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B99" s="5" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="C99" s="8"/>
       <c r="D99" s="8" t="s">
-        <v>6</v>
+        <v>308</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>84</v>
+        <v>366</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A101" s="11"/>
-      <c r="B101" s="12"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102" s="12"/>
-      <c r="B102" s="12"/>
+      <c r="A101" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.1640625" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>85</v>
+        <v>367</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>86</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>89</v>
+      <c r="A2" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>91</v>
+      <c r="A3" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>92</v>
+      <c r="A4" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>94</v>
+      <c r="A5" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>95</v>
+      <c r="A6" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>96</v>
+      <c r="A7" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>97</v>
+      <c r="A8" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>98</v>
+      <c r="A9" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>99</v>
+      <c r="A10" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>100</v>
+      <c r="A11" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>369</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>370</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>371</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>102</v>
+        <v>372</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>373</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>374</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>375</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>376</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>377</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B20" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <autoFilter ref="A1:B20" xr:uid="{00000000-0009-0000-0000-000003000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B20">
       <sortCondition descending="1" ref="B1:B20"/>
     </sortState>
@@ -1719,79 +4397,74 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C6"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.6640625" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="116.5" customWidth="1"/>
+    <col min="3" max="3" width="141" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>378</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>109</v>
+        <v>45</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>110</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>111</v>
+      <c r="A2" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>380</v>
       </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>382</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>384</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>118</v>
+      <c r="A5" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>386</v>
       </c>
       <c r="C5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" t="s">
-        <v>122</v>
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -1799,8 +4472,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1815,33 +4488,33 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>128</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>390</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>391</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>392</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>